<commit_message>
Added a comment for one of the data values
</commit_message>
<xml_diff>
--- a/Wall Clock Sort Times.xlsx
+++ b/Wall Clock Sort Times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Downloads\practice-assignment-04-secretbetta-master\practice-assignment-04-secretbetta-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0D4ABDF-DC5B-4BF6-9869-DE4C01C1B79D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C78391C1-465C-4572-B710-F8BC00B586D2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{F6D450ED-F9CB-4CC7-B81A-FFDDE8666C20}"/>
   </bookViews>
@@ -22,6 +22,40 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Andrew</author>
+  </authors>
+  <commentList>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{50B8AE4A-931E-4666-8D8D-C351C691B8FF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andrew:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This 708 second test time could be a result of running the test and then closing my laptop because I was leaving the Bart train.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +104,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1585,15 +1632,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>205740</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1805940</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>762000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1917,11 +1964,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6AB9AB-1D1D-41E5-B11C-47DAEEA4A534}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6AB9AB-1D1D-41E5-B11C-47DAEEA4A534}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1930,6 +1977,7 @@
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
     <col min="3" max="3" width="25.21875" customWidth="1"/>
     <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="108.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1942,7 +1990,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1"/>
@@ -1953,7 +2001,7 @@
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -1962,7 +2010,7 @@
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2122,7 +2170,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
     </row>
-    <row r="15" spans="1:5" ht="225" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
@@ -2192,7 +2240,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="346.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2203,5 +2251,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>